<commit_message>
Improve colors and legend arrangement. Add link to fact sheet in SharePoint.
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="70">
   <si>
     <t>TileID</t>
   </si>
@@ -61,10 +61,13 @@
     <t>TBD-Shares</t>
   </si>
   <si>
+    <t>Region</t>
+  </si>
+  <si>
     <t>County</t>
   </si>
   <si>
-    <t>Region</t>
+    <t>15-County Region</t>
   </si>
   <si>
     <t>Delaware County</t>
@@ -112,12 +115,12 @@
     <t>Union County</t>
   </si>
   <si>
-    <t>15-County Region</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/employment-industry/refs/heads/main/output_data/charts/shares-Region15.svg</t>
+  </si>
+  <si>
     <t>https://raw.githubusercontent.com/morpc-insights/employment-industry/refs/heads/main/output_data/charts/shares-Delaware.svg</t>
   </si>
   <si>
@@ -163,9 +166,6 @@
     <t>https://raw.githubusercontent.com/morpc-insights/employment-industry/refs/heads/main/output_data/charts/shares-Union.svg</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/morpc-insights/employment-industry/refs/heads/main/output_data/charts/shares-Region15.svg</t>
-  </si>
-  <si>
     <t>Mid-Ohio Regional Planning Commission</t>
   </si>
   <si>
@@ -175,6 +175,9 @@
     <t>annually</t>
   </si>
   <si>
+    <t>https://www.arcgis.com/apps/dashboards/f939956abd634937b0e875b7a277aec9#region=15-County%20Region</t>
+  </si>
+  <si>
     <t>https://www.arcgis.com/apps/dashboards/f939956abd634937b0e875b7a277aec9#region=Delaware%20County</t>
   </si>
   <si>
@@ -220,7 +223,7 @@
     <t>https://www.arcgis.com/apps/dashboards/f939956abd634937b0e875b7a277aec9#region=Union%20County</t>
   </si>
   <si>
-    <t>https://www.arcgis.com/apps/dashboards/f939956abd634937b0e875b7a277aec9#region=15-County%20Region</t>
+    <t>https://morpc1-my.sharepoint.com/:w:/g/personal/aporr_morpc_org/EZcbpRmm-OVAloxLS3ZdKuIBEXDlLLfcxc66yA4282nWaA?e=DL4oZ1</t>
   </si>
 </sst>
 </file>
@@ -672,13 +675,16 @@
       <c r="M2" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="N2" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -704,13 +710,16 @@
       <c r="M3" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="N3" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -736,13 +745,16 @@
       <c r="M4" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="N4" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -768,13 +780,16 @@
       <c r="M5" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="N5" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -800,13 +815,16 @@
       <c r="M6" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="N6" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -832,13 +850,16 @@
       <c r="M7" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="N7" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -864,13 +885,16 @@
       <c r="M8" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="N8" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -896,13 +920,16 @@
       <c r="M9" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="N9" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -928,13 +955,16 @@
       <c r="M10" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="N10" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
@@ -960,13 +990,16 @@
       <c r="M11" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="N11" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
         <v>27</v>
@@ -992,13 +1025,16 @@
       <c r="M12" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="N12" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -1024,13 +1060,16 @@
       <c r="M13" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="N13" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
@@ -1056,13 +1095,16 @@
       <c r="M14" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="N14" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:14">
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>30</v>
@@ -1088,13 +1130,16 @@
       <c r="M15" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="N15" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
@@ -1120,8 +1165,11 @@
       <c r="M16" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="2:13">
+      <c r="N16" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1151,42 +1199,61 @@
       </c>
       <c r="M17" s="2" t="s">
         <v>68</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2" location="region=Delaware%20County"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="M3" r:id="rId4" location="region=Fairfield%20County"/>
-    <hyperlink ref="H4" r:id="rId5"/>
-    <hyperlink ref="M4" r:id="rId6" location="region=Fayette%20County"/>
-    <hyperlink ref="H5" r:id="rId7"/>
-    <hyperlink ref="M5" r:id="rId8" location="region=Franklin%20County"/>
-    <hyperlink ref="H6" r:id="rId9"/>
-    <hyperlink ref="M6" r:id="rId10" location="region=Hocking%20County"/>
-    <hyperlink ref="H7" r:id="rId11"/>
-    <hyperlink ref="M7" r:id="rId12" location="region=Knox%20County"/>
-    <hyperlink ref="H8" r:id="rId13"/>
-    <hyperlink ref="M8" r:id="rId14" location="region=Licking%20County"/>
-    <hyperlink ref="H9" r:id="rId15"/>
-    <hyperlink ref="M9" r:id="rId16" location="region=Logan%20County"/>
-    <hyperlink ref="H10" r:id="rId17"/>
-    <hyperlink ref="M10" r:id="rId18" location="region=Madison%20County"/>
-    <hyperlink ref="H11" r:id="rId19"/>
-    <hyperlink ref="M11" r:id="rId20" location="region=Marion%20County"/>
-    <hyperlink ref="H12" r:id="rId21"/>
-    <hyperlink ref="M12" r:id="rId22" location="region=Morrow%20County"/>
-    <hyperlink ref="H13" r:id="rId23"/>
-    <hyperlink ref="M13" r:id="rId24" location="region=Perry%20County"/>
-    <hyperlink ref="H14" r:id="rId25"/>
-    <hyperlink ref="M14" r:id="rId26" location="region=Pickaway%20County"/>
-    <hyperlink ref="H15" r:id="rId27"/>
-    <hyperlink ref="M15" r:id="rId28" location="region=Ross%20County"/>
-    <hyperlink ref="H16" r:id="rId29"/>
-    <hyperlink ref="M16" r:id="rId30" location="region=Union%20County"/>
-    <hyperlink ref="H17" r:id="rId31"/>
-    <hyperlink ref="M17" r:id="rId32" location="region=15-County%20Region"/>
+    <hyperlink ref="M2" r:id="rId2" location="region=15-County%20Region"/>
+    <hyperlink ref="N2" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="M3" r:id="rId5" location="region=Delaware%20County"/>
+    <hyperlink ref="N3" r:id="rId6"/>
+    <hyperlink ref="H4" r:id="rId7"/>
+    <hyperlink ref="M4" r:id="rId8" location="region=Fairfield%20County"/>
+    <hyperlink ref="N4" r:id="rId9"/>
+    <hyperlink ref="H5" r:id="rId10"/>
+    <hyperlink ref="M5" r:id="rId11" location="region=Fayette%20County"/>
+    <hyperlink ref="N5" r:id="rId12"/>
+    <hyperlink ref="H6" r:id="rId13"/>
+    <hyperlink ref="M6" r:id="rId14" location="region=Franklin%20County"/>
+    <hyperlink ref="N6" r:id="rId15"/>
+    <hyperlink ref="H7" r:id="rId16"/>
+    <hyperlink ref="M7" r:id="rId17" location="region=Hocking%20County"/>
+    <hyperlink ref="N7" r:id="rId18"/>
+    <hyperlink ref="H8" r:id="rId19"/>
+    <hyperlink ref="M8" r:id="rId20" location="region=Knox%20County"/>
+    <hyperlink ref="N8" r:id="rId21"/>
+    <hyperlink ref="H9" r:id="rId22"/>
+    <hyperlink ref="M9" r:id="rId23" location="region=Licking%20County"/>
+    <hyperlink ref="N9" r:id="rId24"/>
+    <hyperlink ref="H10" r:id="rId25"/>
+    <hyperlink ref="M10" r:id="rId26" location="region=Logan%20County"/>
+    <hyperlink ref="N10" r:id="rId27"/>
+    <hyperlink ref="H11" r:id="rId28"/>
+    <hyperlink ref="M11" r:id="rId29" location="region=Madison%20County"/>
+    <hyperlink ref="N11" r:id="rId30"/>
+    <hyperlink ref="H12" r:id="rId31"/>
+    <hyperlink ref="M12" r:id="rId32" location="region=Marion%20County"/>
+    <hyperlink ref="N12" r:id="rId33"/>
+    <hyperlink ref="H13" r:id="rId34"/>
+    <hyperlink ref="M13" r:id="rId35" location="region=Morrow%20County"/>
+    <hyperlink ref="N13" r:id="rId36"/>
+    <hyperlink ref="H14" r:id="rId37"/>
+    <hyperlink ref="M14" r:id="rId38" location="region=Perry%20County"/>
+    <hyperlink ref="N14" r:id="rId39"/>
+    <hyperlink ref="H15" r:id="rId40"/>
+    <hyperlink ref="M15" r:id="rId41" location="region=Pickaway%20County"/>
+    <hyperlink ref="N15" r:id="rId42"/>
+    <hyperlink ref="H16" r:id="rId43"/>
+    <hyperlink ref="M16" r:id="rId44" location="region=Ross%20County"/>
+    <hyperlink ref="N16" r:id="rId45"/>
+    <hyperlink ref="H17" r:id="rId46"/>
+    <hyperlink ref="M17" r:id="rId47" location="region=Union%20County"/>
+    <hyperlink ref="N17" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>